<commit_message>
Replaced all files with the latest  v2 version from local GRP_Project
</commit_message>
<xml_diff>
--- a/data_notes.xlsx
+++ b/data_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andyburnett/Library/Mobile Documents/com~apple~CloudDocs/Desktop/X_12.18.2024/Education/Graduate/USF Grad/Classes/SP25/ISM6137_StatsDM/GRP_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12B8F479-C071-8D4A-9D72-01CBBECB2EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D432CF73-4A16-224C-BA9F-643E2D6DC8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37820" yWindow="500" windowWidth="30100" windowHeight="26800" activeTab="1" xr2:uid="{83C755BF-01C1-854F-B6A1-7D7D9B1DBE15}"/>
+    <workbookView xWindow="32420" yWindow="500" windowWidth="34040" windowHeight="26800" activeTab="1" xr2:uid="{83C755BF-01C1-854F-B6A1-7D7D9B1DBE15}"/>
   </bookViews>
   <sheets>
     <sheet name="ERD" sheetId="1" r:id="rId1"/>
@@ -1229,10 +1229,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B06E7997-C01C-844E-ADAE-8DBBDA6C4E52}">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1241,6 +1241,7 @@
     <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="1.83203125" style="29" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="22"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.1640625" bestFit="1" customWidth="1"/>
@@ -2190,14 +2191,12 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C30" s="37"/>
-      <c r="D30" s="21"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C31" s="37"/>
-      <c r="D31" s="21"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C32" s="37"/>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H36" s="23"/>
+    </row>
+    <row r="37" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H37" s="23"/>
     </row>
     <row r="38" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H38" s="23"/>
@@ -2212,17 +2211,11 @@
       <c r="H41" s="23"/>
     </row>
     <row r="42" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H42" s="23"/>
-    </row>
-    <row r="43" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H43" s="23"/>
-    </row>
-    <row r="44" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H44" s="24"/>
+      <c r="H42" s="24"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L54">
-    <sortCondition ref="J1:J54"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L52">
+    <sortCondition ref="J1:J52"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>